<commit_message>
Update moodman evidence.xlsx for Task A1-A6
</commit_message>
<xml_diff>
--- a/Boblev999/evidence.xlsx
+++ b/Boblev999/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="50">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -124,52 +124,55 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">C0F760B24171DF7FFCE02EE0DCE3D2758582FE701BE8229981E7927C8F5B37AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moodmanGoN</t>
+    <t xml:space="preserve">9B4462857AA65C068537F0A8ED8EC7473D93DD3A7ED595C040C0245C817DBCD9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moodmanftGoN</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">C5115336BDE7F4F92DA10BD39160E546236D33B252CF4A980ED165045072F2AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F81DD479B9B98958F1A68FB367D855BA2B6E53A0DFD6C06B4974A749428B1E63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moodmanGoN1</t>
+    <t xml:space="preserve">D9CA5A959A038D31DDAB2402DF86EF1835BD24268CDFE8A3D0B706F0F7C6D6E9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moodmanftGoN001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A02001BFD0D0910BD3F6ABCBD14B1D8B3EB8650521E8626D0CC01711C91612B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moodmanftGoN002</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">874B01F238987BA3D856DDF747729DFE05798E70FBFE25CFCDD60E3203D2E2FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wasm.juno1f9de2udw65wy7n7fh3tvd3n463xrppsgcjyrzcp5mj2l6czyuvwsk3zsmy</t>
+    <t xml:space="preserve">DC3C49E5C8EA91FFC3A0A30EFD0EE26201662BADFD05AF454CC1DF2762682B71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasm.juno17vuqemwzsten4nu02x5m0se9uecagvvhusd7zy8nu5kzp5uq4l8q5s5c4l</t>
   </si>
   <si>
     <t xml:space="preserve">JUNO</t>
   </si>
   <si>
-    <t xml:space="preserve">813DAA2E3763D8386133188CB2890875E5BB693EC980B05D8D98D1928BFB501D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc/AB1B881C808A7B71F998DC3E5A36AA09DF2B94F6EF3FB7BBBBF7DA7732B44DFD</t>
+    <t xml:space="preserve">E2FFD638D68C314C508A4A70E29DBA1E18809F87BD8A10E0534F65E6E64D1BF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/CA425961110206E9CEC482A6AA7F668D66773F379EF47020FE6D8827F6784035</t>
   </si>
   <si>
     <t xml:space="preserve">UPTICK</t>
   </si>
   <si>
-    <t xml:space="preserve">B4CC7EC780C1C3C67D82DBB0BAD1EF6B636FD047D2EE0DFC494F5A6770BC7968</t>
+    <t xml:space="preserve">27A42F7421E1F17BD6D9436ABEE81A5F565151405AEFC5204EABBE774ADA675B</t>
   </si>
   <si>
     <t xml:space="preserve">IRIS</t>
   </si>
   <si>
-    <t xml:space="preserve">7857F23DDF69AA0514C21552738FAC14BFD9D02B79BB83F88E4E562AC2BA84EE</t>
+    <t xml:space="preserve">F11C46AB03E0C460BE1CBDCDF02F26D2ECFEC8F5FEDA24B18DAC0242CE9B820E</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
@@ -536,11 +539,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -579,11 +582,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -622,11 +625,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -665,11 +668,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -703,439 +706,439 @@
         <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1169,12 +1172,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1208,12 +1211,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1247,12 +1250,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1286,12 +1289,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1341,18 +1344,18 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1377,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1394,21 +1397,21 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1433,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1450,21 +1453,21 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1489,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1506,21 +1509,21 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1541,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,22 +1567,22 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1618,11 +1621,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1661,11 +1664,11 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
A1-A6  fix - sender not match register address
</commit_message>
<xml_diff>
--- a/Boblev999/evidence.xlsx
+++ b/Boblev999/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -70,30 +70,6 @@
     <t xml:space="preserve">Community</t>
   </si>
   <si>
-    <t xml:space="preserve">team name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addr5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discord#1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set none if no community</t>
-  </si>
-  <si>
     <t xml:space="preserve">moodman</t>
   </si>
   <si>
@@ -113,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">diboss || moodman#1246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">TxHash</t>
@@ -400,8 +379,8 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,41 +447,63 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -520,32 +521,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -563,32 +564,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -606,37 +607,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -649,71 +650,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -745,28 +703,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -798,28 +756,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -851,28 +809,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -904,28 +862,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -957,28 +915,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1010,71 +968,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1106,28 +1064,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1156,17 +1114,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1195,17 +1153,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1234,17 +1192,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1273,17 +1231,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1316,35 +1274,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1377,30 +1335,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1433,30 +1391,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1489,30 +1447,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1491,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1547,31 +1505,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1602,18 +1560,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1645,18 +1603,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>